<commit_message>
[22 12a] add excel_zad1.ipynb
</commit_message>
<xml_diff>
--- a/day22_15_02_2026/sample.xlsx
+++ b/day22_15_02_2026/sample.xlsx
@@ -1,41 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radoslawjaniak/BootCamp-11-10-2025-DATA/day22_15_02_2026/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924273AB-85A8-4C41-8E9C-BF4B97BF3A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-22540" yWindow="-10600" windowWidth="29400" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -54,22 +49,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -357,35 +411,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="1">
+      <c r="A1" t="n">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>46068.535327179983</v>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>46068.56307746364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>